<commit_message>
excel uploading api,horse details addig method and race creation completed
</commit_message>
<xml_diff>
--- a/public/race.xlsx
+++ b/public/race.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Race 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="47">
   <si>
     <t xml:space="preserve">HorseNumber</t>
   </si>
@@ -163,9 +163,6 @@
   </si>
   <si>
     <t xml:space="preserve">K Sunny Kumar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AgeColorSex</t>
   </si>
 </sst>
 </file>
@@ -383,7 +380,7 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
@@ -394,7 +391,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="7.44"/>
@@ -812,13 +809,13 @@
   </sheetPr>
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
+      <selection pane="bottomLeft" activeCell="P19" activeCellId="0" sqref="P19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.92"/>
@@ -840,7 +837,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>4</v>
@@ -1160,7 +1157,7 @@
       <selection pane="bottomRight" activeCell="F28" activeCellId="0" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.92"/>

</xml_diff>